<commit_message>
Se modificó el tamaño de la celda en la tabla exportada con spreedsheet. Se cambió el tooltip del index al realizar una búsqueda, aclarando que se exporta, no la lista actual sino los tickets abiertos que se muestran en la tabla de index. Se removieron los comentarios de chat gpt Se agregó el decorador para autenticar al usuario, es la operación número 40. (se hicieron pruebas modificando la Base de datos, agregando la operación Exportar_Tickets y dándole acceso a los roles 1 y 2) Se agregaron los logs al método, guarda el nombre de quien exportó la tabla y el número de tickets que se exportaron en los Logs de Tickets. Se corrigió el bug que guardaba la tabla exportada diariamente. Ahora se usa MemoryStream para poder guardar en el archivo en memoria en vez del servidor cada que se descarga, así no llenará el almacenamiento.
</commit_message>
<xml_diff>
--- a/Prototipo_Tabla/Lista_de_tickets_.xlsx
+++ b/Prototipo_Tabla/Lista_de_tickets_.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dulce\source\repos\julianMondragon\TAS360\Prototipo_Tabla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81E2A82-F824-47A2-AE21-B28214E5437D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D42317-6BCB-4353-AA31-072869B65CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,7 +98,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -114,6 +114,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -479,22 +485,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1995" topLeftCell="A8" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2850" topLeftCell="A8"/>
+      <selection activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="45.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="78.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20" style="2" customWidth="1"/>
+    <col min="7" max="9" width="12.7109375" style="2" customWidth="1"/>
     <col min="10" max="10" width="13.42578125" style="1" customWidth="1"/>
     <col min="11" max="11" width="10.140625" style="1" customWidth="1"/>
     <col min="12" max="12" width="18" style="1" customWidth="1"/>
@@ -505,34 +510,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="E3" s="7" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="E3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
     </row>
     <row r="7" spans="1:10" s="4" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -563,7 +568,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="6"/>
+      <c r="C8" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:C5"/>

</xml_diff>